<commit_message>
Includes 4 more functions
</commit_message>
<xml_diff>
--- a/Original_Data/Text Methods.xlsx
+++ b/Original_Data/Text Methods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanch\Documents\GitHub_Excel\Original_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44550022-9846-46AD-9534-1758A8D6AB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584B6CDE-38AA-4027-8266-587E9CEA6565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C627DCA1-2D43-4E79-826D-EF32120C3259}"/>
   </bookViews>
@@ -17,6 +17,8 @@
     <sheet name="CONCAT" sheetId="4" r:id="rId2"/>
     <sheet name="Upper,Lower,Proper" sheetId="1" r:id="rId3"/>
     <sheet name="TRIM" sheetId="2" r:id="rId4"/>
+    <sheet name="Replace And Substitute" sheetId="5" r:id="rId5"/>
+    <sheet name="FIND and SEARCH" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
   <si>
     <t>Last Name</t>
   </si>
@@ -191,6 +193,45 @@
   </si>
   <si>
     <t>ram</t>
+  </si>
+  <si>
+    <t>27-Jan-2022 = 27 January 2022</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>Replace</t>
+  </si>
+  <si>
+    <t>Substitue</t>
+  </si>
+  <si>
+    <t>Bhide Minocha</t>
+  </si>
+  <si>
+    <t>Ghanshyam Ramesh</t>
+  </si>
+  <si>
+    <t>Ramesh Balram</t>
+  </si>
+  <si>
+    <t>Ghanshyam Arjun</t>
+  </si>
+  <si>
+    <t>Ghanshyam Ram</t>
+  </si>
+  <si>
+    <t>Bhide Ghanshyam</t>
+  </si>
+  <si>
+    <t>Laxman Shyam</t>
+  </si>
+  <si>
+    <t>Ramesh Bhide</t>
+  </si>
+  <si>
+    <t>Laxman Bhide</t>
   </si>
 </sst>
 </file>
@@ -228,7 +269,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -322,11 +363,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -346,6 +418,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,7 +739,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -833,7 +909,7 @@
   <dimension ref="A3:N13"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -878,15 +954,15 @@
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="str">
         <f t="shared" ref="A5:B13" ca="1" si="0">INDEX($M$5:$M$13,RANDBETWEEN(1,9))</f>
-        <v>ramesh</v>
+        <v>shyam</v>
       </c>
       <c r="B5" s="5" t="str">
         <f ca="1">INDEX($N$5:$N$13,RANDBETWEEN(1,9))</f>
-        <v>gupta</v>
+        <v>mehta</v>
       </c>
       <c r="C5" s="5" t="str">
         <f t="shared" ref="C5:C13" ca="1" si="1">_xlfn.CONCAT(A5," ",B5)</f>
-        <v>ramesh gupta</v>
+        <v>shyam mehta</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -905,11 +981,11 @@
       </c>
       <c r="B6" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>ghanshyam</v>
+        <v>balram</v>
       </c>
       <c r="C6" s="5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>laxman ghanshyam</v>
+        <v>laxman balram</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -924,15 +1000,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
+        <v>laxman</v>
+      </c>
+      <c r="B7" s="5" t="str">
+        <f t="shared" ca="1" si="0"/>
         <v>bhavesh</v>
-      </c>
-      <c r="B7" s="5" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>bhide</v>
       </c>
       <c r="C7" s="5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>bhavesh bhide</v>
+        <v>laxman bhavesh</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -947,15 +1023,15 @@
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>laxman</v>
+        <v>arjun</v>
       </c>
       <c r="B8" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>bhide</v>
+        <v>balram</v>
       </c>
       <c r="C8" s="5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>laxman bhide</v>
+        <v>arjun balram</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -970,15 +1046,15 @@
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>balram</v>
+        <v>ghanshyam</v>
       </c>
       <c r="B9" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>laxman</v>
+        <v>bhavesh</v>
       </c>
       <c r="C9" s="5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>balram laxman</v>
+        <v>ghanshyam bhavesh</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
@@ -993,15 +1069,15 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>ghanshyam</v>
+        <v>laxman</v>
       </c>
       <c r="B10" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>shyam</v>
+        <v>balram</v>
       </c>
       <c r="C10" s="5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ghanshyam shyam</v>
+        <v>laxman balram</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -1016,15 +1092,15 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>ram</v>
+        <v>ghanshyam</v>
       </c>
       <c r="B11" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>ramesh</v>
+        <v>bhide</v>
       </c>
       <c r="C11" s="5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ram ramesh</v>
+        <v>ghanshyam bhide</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -1043,11 +1119,11 @@
       </c>
       <c r="B12" s="5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>ghanshyam</v>
+        <v>bhavesh</v>
       </c>
       <c r="C12" s="5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>arjun ghanshyam</v>
+        <v>arjun bhavesh</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -1062,15 +1138,15 @@
     <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>ghanshyam</v>
+        <v>ram</v>
       </c>
       <c r="B13" s="6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>balram</v>
+        <v>bhavesh</v>
       </c>
       <c r="C13" s="6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ghanshyam balram</v>
+        <v>ram bhavesh</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -1166,4 +1242,130 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A29F6A1-DB78-4A23-ACBD-5786F199BA2F}">
+  <dimension ref="B3:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ACC1ED4-2B52-4072-941A-83ACE0BFC60F}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.109375" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="20"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>